<commit_message>
ExportResults fixed to accept custom path
</commit_message>
<xml_diff>
--- a/dropsApiTest.xlsx
+++ b/dropsApiTest.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C0ED30-75B7-2F48-9D2F-FAA0A6C0DB6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73F443D-DC1E-454D-A787-CB7BE336A727}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31640" yWindow="1960" windowWidth="28240" windowHeight="17560" xr2:uid="{C078BFE5-CB95-AB43-9140-1B62DB89791E}"/>
+    <workbookView xWindow="-37360" yWindow="1960" windowWidth="18300" windowHeight="17560" xr2:uid="{C078BFE5-CB95-AB43-9140-1B62DB89791E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Testcases" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>baseURL</t>
   </si>
@@ -55,13 +55,28 @@
   </si>
   <si>
     <t>[{"baseURL": "https://app-eu.earthsquad.global/api/rest-auth/login/","Username":"test151","Password":"bb140272!"}]</t>
+  </si>
+  <si>
+    <t>TFName</t>
+  </si>
+  <si>
+    <t>TFDescription</t>
+  </si>
+  <si>
+    <t>Login 1</t>
+  </si>
+  <si>
+    <t>Login 2</t>
+  </si>
+  <si>
+    <t>Login with Username and Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -76,6 +91,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF008080"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,9 +121,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -417,60 +440,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1771157A-AD36-4846-BB39-339247F0A5E3}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{BCA73E9C-2662-9740-B28A-F40781884EC3}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{1624A2E0-3017-A24C-8BEF-52F734638001}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{BCA73E9C-2662-9740-B28A-F40781884EC3}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{1624A2E0-3017-A24C-8BEF-52F734638001}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>